<commit_message>
Updated for better page selection
All of november
</commit_message>
<xml_diff>
--- a/pagespeed-results_24112015.xlsx
+++ b/pagespeed-results_24112015.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="240" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="pagespeed-results.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="24 Nov 2015" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'24 Nov 2015'!$A$1:$T$175</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="365">
   <si>
     <t>URL</t>
   </si>
@@ -1105,13 +1108,32 @@
   </si>
   <si>
     <t>Page speed test - 24 Nov 2015</t>
+  </si>
+  <si>
+    <t>Means</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1149,6 +1171,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1173,26 +1209,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1521,11 +1583,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T172"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A172"/>
+      <pane ySplit="3" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L175" sqref="L175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1534,6 +1599,11 @@
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="30">
@@ -12083,15 +12153,241 @@
         <v>0</v>
       </c>
     </row>
+    <row r="173" spans="1:20" s="3" customFormat="1">
+      <c r="B173" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E173" s="4">
+        <f>AVERAGE(E4:E172)</f>
+        <v>1.8456004931005912</v>
+      </c>
+      <c r="G173" s="5">
+        <f>AVERAGE(G4:G172)</f>
+        <v>84.798816568047343</v>
+      </c>
+      <c r="H173" s="5"/>
+      <c r="I173" s="5">
+        <f t="shared" ref="I173:T173" si="0">AVERAGE(I4:I172)</f>
+        <v>3358.3017751479292</v>
+      </c>
+      <c r="J173" s="5"/>
+      <c r="K173" s="5"/>
+      <c r="L173" s="5">
+        <f t="shared" si="0"/>
+        <v>513667.65680473374</v>
+      </c>
+      <c r="M173" s="5"/>
+      <c r="N173" s="5"/>
+      <c r="O173" s="5">
+        <f t="shared" si="0"/>
+        <v>22609.781065088759</v>
+      </c>
+      <c r="P173" s="5">
+        <f t="shared" si="0"/>
+        <v>39562.065088757394</v>
+      </c>
+      <c r="Q173" s="5"/>
+      <c r="R173" s="5">
+        <f t="shared" si="0"/>
+        <v>308796.05325443787</v>
+      </c>
+      <c r="T173" s="5">
+        <f t="shared" si="0"/>
+        <v>898.41420118343194</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20">
+      <c r="B174" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E174" s="6">
+        <f>MAX(E4:E172)/E173-1</f>
+        <v>5.998264276740219</v>
+      </c>
+      <c r="G174" s="6">
+        <f>MAX(G4:G172)/G173-1</f>
+        <v>1.4165096643639519E-2</v>
+      </c>
+      <c r="H174" s="3"/>
+      <c r="I174" s="6">
+        <f>MAX(I4:I172)/I173-1</f>
+        <v>0.9557503880694842</v>
+      </c>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+      <c r="L174" s="6">
+        <f>MAX(L4:L172)/L173-1</f>
+        <v>0.92129480399651498</v>
+      </c>
+      <c r="M174" s="3"/>
+      <c r="N174" s="3"/>
+      <c r="O174" s="6">
+        <f>MAX(O4:O172)/O173-1</f>
+        <v>2.9820376739082128</v>
+      </c>
+      <c r="P174" s="6">
+        <f>MAX(P4:P172)/P173-1</f>
+        <v>24.036913461867798</v>
+      </c>
+      <c r="Q174" s="3"/>
+      <c r="R174" s="6">
+        <f>MAX(R4:R172)/R173-1</f>
+        <v>4.3380863603259483</v>
+      </c>
+      <c r="T174" s="6">
+        <f>MAX(T4:T172)/T173-1</f>
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:20">
+      <c r="B175" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E175" s="6">
+        <f>MIN(E4:E172)/E173-1</f>
+        <v>-1</v>
+      </c>
+      <c r="G175" s="6">
+        <f>MIN(G4:G172)/G173-1</f>
+        <v>-0.12734631219035664</v>
+      </c>
+      <c r="H175" s="3"/>
+      <c r="I175" s="6">
+        <f>MIN(I4:I172)/I173-1</f>
+        <v>-0.14718801592098008</v>
+      </c>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+      <c r="L175" s="6">
+        <f>MIN(L4:L172)/L173-1</f>
+        <v>-0.28409936828124793</v>
+      </c>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
+      <c r="O175" s="6">
+        <f>MIN(O4:O172)/O173-1</f>
+        <v>-0.31370410198445298</v>
+      </c>
+      <c r="P175" s="6">
+        <f>MIN(P4:P172)/P173-1</f>
+        <v>-0.72003483703009374</v>
+      </c>
+      <c r="Q175" s="3"/>
+      <c r="R175" s="6">
+        <f>MIN(R4:R172)/R173-1</f>
+        <v>-0.25591341735615969</v>
+      </c>
+      <c r="T175" s="6">
+        <f>MIN(T4:T172)/T173-1</f>
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B4:T172">
     <sortCondition descending="1" ref="E4:E172"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="E4:E172">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G172">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I172">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L172">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O172">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P172">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R172">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T172">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="8" scale="64" fitToHeight="3" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>